<commit_message>
Added websites to json
</commit_message>
<xml_diff>
--- a/learning-files/list-of-licenses.xlsx
+++ b/learning-files/list-of-licenses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Bootcamp\challenge-questions-and-projects\challenge-question-9\gato365P-readme-generator\learning-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2B07CE1-E627-4D61-9191-3BAEB1453C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150CF623-573F-4066-B9C5-97A7D039198D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{06D9D847-0451-456A-B3CB-7DADED64C2E2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="88">
   <si>
     <t>Academic Free License v3.0</t>
   </si>
@@ -246,13 +246,67 @@
   </si>
   <si>
     <t>license-name</t>
+  </si>
+  <si>
+    <t>license-website</t>
+  </si>
+  <si>
+    <t>https://opensource.org/licenses/Apache-2.0</t>
+  </si>
+  <si>
+    <t>https://www.boost.org/LICENSE_1_0.txt</t>
+  </si>
+  <si>
+    <t>https://opensource.org/licenses/BSD-3-Clause</t>
+  </si>
+  <si>
+    <t>https://opensource.org/licenses/BSD-2-Clause</t>
+  </si>
+  <si>
+    <t>http://creativecommons.org/publicdomain/zero/1.0/</t>
+  </si>
+  <si>
+    <t>https://creativecommons.org/licenses/by/4.0/</t>
+  </si>
+  <si>
+    <t>https://licensebuttons.net/l/by-sa/4.0/80x15.png)](https://creativecommons.org/licenses/by-sa/4.0/</t>
+  </si>
+  <si>
+    <t>https://opensource.org/licenses/EPL-1.0</t>
+  </si>
+  <si>
+    <t>https://www.gnu.org/licenses/gpl-3.0</t>
+  </si>
+  <si>
+    <t>https://www.gnu.org/licenses/agpl-3.0</t>
+  </si>
+  <si>
+    <t>https://www.gnu.org/licenses/fdl-1.3</t>
+  </si>
+  <si>
+    <t>https://opensource.org/licenses/ISC</t>
+  </si>
+  <si>
+    <t>https://opensource.org/licenses/MIT</t>
+  </si>
+  <si>
+    <t>https://opensource.org/licenses/MPL-2.0</t>
+  </si>
+  <si>
+    <t>https://opendatacommons.org/licenses/by/</t>
+  </si>
+  <si>
+    <t>https://opensource.org/licenses/Artistic-2.0</t>
+  </si>
+  <si>
+    <t>https://opensource.org/licenses/OFL-1.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,6 +322,12 @@
     </font>
     <font>
       <sz val="14"/>
+      <color rgb="FF24292F"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="7"/>
       <color rgb="FF24292F"/>
       <name val="Consolas"/>
       <family val="3"/>
@@ -314,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -322,6 +382,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -636,294 +698,401 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B40DF5BB-38DA-4B1E-B45F-EC280EFEB2D6}">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="A1:C35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="48.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.7265625" customWidth="1"/>
+    <col min="2" max="2" width="18.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="C1" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="C2" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="C3" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="C4" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="C5" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="C6" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="C7" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="C8" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="C9" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="C10" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="C11" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="C12" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="C13" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="C14" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="C15" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="C16" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="C17" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="C18" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="C19" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="C20" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="C21" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="C22" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="C23" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="C24" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="C25" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="C26" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="C27" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="C28" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="C29" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="C30" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="C31" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="C32" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="C33" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="C34" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>67</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>